<commit_message>
Added functionality to make it so it does lists of lists
</commit_message>
<xml_diff>
--- a/Excel_Data.xlsx
+++ b/Excel_Data.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet0" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -405,7 +407,6 @@
       <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -427,7 +428,6 @@
       <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -449,7 +449,6 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -471,7 +470,906 @@
       <c r="E5" t="n">
         <v>2</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Career</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Computer</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Apache Tomcat - Error report</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/Job/software-engineer-in-test-jobs-SRCH_KO0,25.htm</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Object Oriented Software Developer Jobs, Employment | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/q-Object-Oriented-Software-Developer-jobs.html</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1756</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>45,000+ Software Developer In Test jobs in United States (1,132 new)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/software-developer-in-test-jobs</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>715</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Software Development Engineer in Test Jobs, Employment | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/q-Software-Development-Engineer-in-Test-jobs.html</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1545</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Job Application for Software Engineer in Test at TrueMotion</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/truemotion/jobs/1236070</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>72</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">text@example.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Software Test Engineer Jobs, Employment | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/q-Software-Test-Engineer-jobs.html</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1587</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>14,000+ Software Development Engineer In Test jobs in United States (192 new)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/software-development-engineer-in-test-jobs</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>705</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Software Developer Job Listings | Career Search | Monster.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://www.monster.com/jobs/q-software-developer-jobs</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>499</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Software Development Jobs - Remote, Part-Time &amp; Freelance | FlexJobs</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://www.flexjobs.com/jobs/web-software-development-programming</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>458</v>
+      </c>
+      <c r="D10" t="n">
+        <v>7</v>
+      </c>
+      <c r="E10" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>How to Get a Software Engineer Job at Google and Other Top Tech Companies</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://www.freecodecamp.org/news/how-to-get-a-software-engineer-job-at-google-and-other-top-tech-companies-efa235a33a6d/</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>61</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Software Developer in Test, Lumberyard Quality - Job ID: 843190 | Amazon.jobs</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://www.amazon.jobs/en/jobs/843190/software-developer-in-test-lumberyard-quality</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>104</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Software Developer Jobs with Aerotek</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://www.aerotek.com/en/career-opportunities/engineering-jobs/software-developer-jobs</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>149</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Software Developers: Jobs, Career, Salary and Education Information    </t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://collegegrad.com/careers/software-developers</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>81</v>
+      </c>
+      <c r="D14" t="n">
+        <v>70</v>
+      </c>
+      <c r="E14" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Best Software Engineer Jobs Los Angeles 2019 | Built In Los Angeles</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://www.builtinla.com/guides/best-software-engineer-jobs-los-angeles</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>237</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Important Job Skills for Software Engineers</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://www.thebalancecareers.com/software-engineer-skills-list-2062483</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>267</v>
+      </c>
+      <c r="D16" t="n">
+        <v>15</v>
+      </c>
+      <c r="E16" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Software Developer Job Description | Job Description Examples | TopResume</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://www.topresume.com/career-advice/software-developer-job-description</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>94</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>19</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">name@example.com
+privacy@topresume.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Remote Software Developer Jobs in December 2019</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://remoteok.io/remote-dev-jobs</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>10879</v>
+      </c>
+      <c r="D18" t="n">
+        <v>85</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1602</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@geektastic.com
+talent@tuftandneedle.com
+sentinelhr@sentinel.com
+jobs@wpwhitesecurity.com
+alise.moncure@integratedrental.com
+alise.moncure@integratedrental.com
+</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Career</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Computer</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Apache Tomcat - Error report</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/Job/software-developer-jobs-SRCH_KO0,18.htm</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Software Development Jobs - Remote, Part-Time &amp; Freelance | FlexJobs</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://www.flexjobs.com/jobs/web-software-development-programming</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>452</v>
+      </c>
+      <c r="D3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3" t="n">
+        <v>17</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>What a developer goes through when looking for a second job</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://www.freecodecamp.org/news/what-a-developer-goes-through-when-looking-for-a-second-job-f061c26ffd8f/</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>45</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>9</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Software Developer Job Listings | Career Search | Monster.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.monster.com/jobs/q-software-developer-jobs</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>499</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
       <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Entry Level Software Developer Jobs, Employment | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/q-Entry-Level-Software-Developer-jobs.html</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1806</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>51</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Software Developer Jobs, Employment | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/q-Software-Developer-jobs.html</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1793</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" t="n">
+        <v>38</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>403 Forbidden</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://insights.dice.com/2019/10/14/compaies-hiring-software-developers-engineers/</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Software Developer - Career Rankings, Salary, Reviews and Advice | US News Best Jobs</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://money.usnews.com/careers/best-jobs/software-developer</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1026</v>
+      </c>
+      <c r="D9" t="n">
+        <v>87</v>
+      </c>
+      <c r="E9" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">robin@csadvising.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Best Software Engineer Jobs Denver 2019 | Built In Colorado</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://www.builtincolorado.com/guides/denver-software-jobs-engineers-colorado</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>243</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>47</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>173,000+ Software Developer jobs in United States (3,891 new)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/software-developer-jobs</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>698</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>25</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Software Developers :     Occupational Outlook Handbook: :     U.S. Bureau of Labor Statistics</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://www.bls.gov/ooh/computer-and-information-technology/software-developers.htm</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>75</v>
+      </c>
+      <c r="D12" t="n">
+        <v>110</v>
+      </c>
+      <c r="E12" t="n">
+        <v>42</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>8 Side Income Ideas For Programmers (That Actually Work) - Afternerd</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://www.afternerd.com/blog/side-income-programmers/</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>13</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>This Map Shows Where All the Open Software Engineering Jobs Are in the U.S. | Inc.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://www.inc.com/salvador-rodriguez/act-software-developers-map.html</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>46</v>
+      </c>
+      <c r="D14" t="n">
+        <v>24</v>
+      </c>
+      <c r="E14" t="n">
+        <v>85</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How I landed my post-bootcamp software developer job in just seven weeks - By </t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://hackernoon.com/how-i-landed-my-post-bootcamp-software-developer-job-in-just-seven-weeks-7b213c1bb867</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>54</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>23</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">support@hackernoon.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Remote Software Developer Jobs in December 2019</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://remoteok.io/remote-dev-jobs</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>10879</v>
+      </c>
+      <c r="D16" t="n">
+        <v>85</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1602</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@geektastic.com
+talent@tuftandneedle.com
+sentinelhr@sentinel.com
+jobs@wpwhitesecurity.com
+alise.moncure@integratedrental.com
+alise.moncure@integratedrental.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Software Development Engineers  | Amazon.jobs</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://www.amazon.jobs/en/teams/software-development-engineers-and-managers</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>60</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>14</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>15-1132.00 - Software Developers, Applications</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://www.onetonline.org/link/summary/15-1132.00</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>64</v>
+      </c>
+      <c r="D18" t="n">
+        <v>31</v>
+      </c>
+      <c r="E18" t="n">
+        <v>452</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>What second job do you suggest for a computer programmer? - Quora</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://www.quora.com/What-second-job-do-you-suggest-for-a-computer-programmer</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>182</v>
+      </c>
+      <c r="D19" t="n">
+        <v>82</v>
+      </c>
+      <c r="E19" t="n">
+        <v>5</v>
+      </c>
+      <c r="F19" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Changed excel sheet names to resume file names
</commit_message>
<xml_diff>
--- a/Excel_Data.xlsx
+++ b/Excel_Data.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet0" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BlewerResume.docx" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RinglerShawn_Resume.docx" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -482,7 +482,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,7 +530,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.upwork.com/l/us/c-programmers-in-wa/</t>
+          <t>https://www.upwork.com/hire/c-sharp-developers/</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -546,72 +546,24 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>14 Programming Languages for Mobile App Development - BuildFire</t>
+          <t>netguru_logo</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://buildfire.com/programming-languages-for-mobile-app-development/</t>
+          <t>https://www.netguru.com/blog/python-vs-c-comparison-of-the-programming-language</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">johndoe@example.com
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>programming languages - For what reasons  should I choose C# over Java and C++? - Software Engineering Stack Exchange</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://softwareengineering.stackexchange.com/questions/125712/for-what-reasons-should-i-choose-c-over-java-and-c</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>42</v>
-      </c>
-      <c r="D4" t="n">
-        <v>7</v>
-      </c>
-      <c r="E4" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>netguru_logo</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>https://www.netguru.com/blog/python-vs-c-comparison-of-the-programming-language</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F5" t="inlineStr">
         <is>
           <t xml:space="preserve">hello@netguru.com
 hello@netguru.com
@@ -619,94 +571,158 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Google plus</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://raygun.com/blog/programming-languages/</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>127</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">example@xyz.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>14 Programming Languages for Mobile App Development - BuildFire</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://buildfire.com/programming-languages-for-mobile-app-development/</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>13</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>17</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">johndoe@example.com
+</t>
+        </is>
+      </c>
+    </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Google plus</t>
+          <t>programming languages - For what reasons  should I choose C# over Java and C++? - Software Engineering Stack Exchange</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://raygun.com/blog/programming-languages/</t>
+          <t>https://softwareengineering.stackexchange.com/questions/125712/for-what-reasons-should-i-choose-c-over-java-and-c</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>127</v>
+        <v>42</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">example@xyz.com
-</t>
-        </is>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Up For Grabs</t>
+          <t>Visual Studio for Linux - Developer Community</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://up-for-grabs.net/</t>
+          <t>https://developercommunity.visualstudio.com/idea/360479/visual-studio-for-linux.html</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">shunjid.se@outlook.com
+shunjid.se@outlook.com
+</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>403 Forbidden</t>
+          <t>Up For Grabs</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.beseen.com/tech-jobs/roles/software-developer.html</t>
+          <t>https://up-for-grabs.net/</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Access Denied</t>
+          <t>Remote C++ Jobs in December 2019</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/c-plus-plus-developer-jobs-in-kolkata</t>
+          <t>https://remoteok.io/remote-c-plus-plus-jobs</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>11220</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>775</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@geektastic.com
+jobs@alienskin.com
+schuss@madeinoffice.com
+jobs@komodoplatform.com
+</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -733,89 +749,96 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-	Video Game, Animation, VFX and Software Jobs matching developer in  - CreativeHeads.net
+          <t>Remote Software Developer Jobs in December 2019</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://remoteok.io/remote-dev-jobs</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>11080</v>
+      </c>
+      <c r="D11" t="n">
+        <v>90</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1617</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@geektastic.com
+talent@tuftandneedle.com
+sentinelhr@sentinel.com
+jobs@wpwhitesecurity.com
+alise.moncure@integratedrental.com
+alise.moncure@integratedrental.com
 </t>
         </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>https://www.highendcareers.com/job-search/developer/everywhere/1</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1139</v>
-      </c>
-      <c r="D11" t="n">
-        <v>6</v>
-      </c>
-      <c r="E11" t="n">
-        <v>69</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>codebar.io</t>
+          <t>Access Denied</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://codebar.io/skills/c%23</t>
+          <t>https://www.naukri.com/c-plus-plus-developer-jobs-in-kolkata</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Linux - Wikipedia</t>
+          <t>GitHub - quozd/awesome-dotnet: A collection of awesome .NET libraries, tools, frameworks and software</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://en.wikipedia.org/wiki/Linux</t>
+          <t>https://github.com/quozd/awesome-dotnet</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>163</v>
+        <v>5</v>
       </c>
       <c r="E13" t="n">
-        <v>81</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-	Video Game, Animation, VFX and Software Jobs matching all jobs in  - CreativeHeads.net
-</t>
+          <t>10 Best Freelance Tcp Developers for Hire in Dec 2019 | Arc</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.creativeheads.net/job-search/all-jobs/everywhere/1</t>
+          <t>https://www.codementor.io/tcp-developers</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1006</v>
+        <v>104</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E14" t="n">
-        <v>40</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15">
@@ -976,83 +999,91 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Remote Software Developer Jobs in December 2019</t>
+          <t>Should C# or C++ be chosen for learning Games Programming (consoles)? - Stack Overflow</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://remoteok.io/remote-dev-jobs</t>
+          <t>https://stackoverflow.com/questions/2203093/should-c-sharp-or-c-be-chosen-for-learning-games-programming-consoles</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>11073</v>
+        <v>62</v>
       </c>
       <c r="D16" t="n">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="E16" t="n">
-        <v>1616</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">hello@geektastic.com
-talent@tuftandneedle.com
-sentinelhr@sentinel.com
-jobs@wpwhitesecurity.com
-alise.moncure@integratedrental.com
-alise.moncure@integratedrental.com
-</t>
-        </is>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Rose International – Available Jobs</t>
+          <t xml:space="preserve">
+	Video Game, Animation, VFX and Software Jobs matching cc++java in  - CreativeHeads.net
+</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.roseit.com/hotjobs/QSeriesQProSpreadsheetHotOpn.aspx?AspxAutoDetectCookieSupport=1</t>
+          <t>https://www.highendcareers.com/job-search/ccplusplusjava/everywhere/1</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2759</v>
+        <v>1164</v>
       </c>
       <c r="D17" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E17" t="n">
-        <v>280</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">careersprocessing@roseint.com
-</t>
-        </is>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t xml:space="preserve">
+	Video Game, Animation, VFX and Software Jobs matching technical support in  - CreativeHeads.net
+</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://www.creativeheads.net/job-search/technical-support/everywhere/3</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1036</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t xml:space="preserve">  Available Developer Jobs on HackerEarth  </t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>https://www.hackerearth.com/jobs/hiring/</t>
         </is>
       </c>
-      <c r="C18" t="n">
-        <v>11298</v>
-      </c>
-      <c r="D18" t="n">
+      <c r="C19" t="n">
+        <v>11299</v>
+      </c>
+      <c r="D19" t="n">
         <v>46</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E19" t="n">
         <v>856</v>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t xml:space="preserve">contact@hackerearth.com
 contact@hackerearth.com
@@ -1136,118 +1167,118 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Top 10 Programming Languages of the World – 2019 to begin with… - GeeksforGeeks</t>
+          <t>Warning: Your programming career - SoloLearn - Medium</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.geeksforgeeks.org/top-10-programming-languages-of-the-world-2019-to-begin-with/</t>
+          <t>https://medium.com/sololearn/warning-your-programming-career-b9579b3a878b</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="D3" t="n">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="E3" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>twitter logo</t>
+          <t>What Programming Language Should a Beginner Learn in 2019? | Codementor</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://dev.to/javinpaul/top-5-programming-languages-every-software-developer-should-learn-3o3o</t>
+          <t>https://www.codementor.io/codementorteam/beginner-programming-language-job-salary-community-7s26wmbm6</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>The 7 Most In-Demand Programming Languages of 2019 - Coding Dojo Blog</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.codingdojo.com/blog/the-7-most-in-demand-programming-languages-of-2019</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>59</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>11</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Top 10 Programming Languages of the World – 2019 to begin with… - GeeksforGeeks</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.geeksforgeeks.org/top-10-programming-languages-of-the-world-2019-to-begin-with/</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>28</v>
+      </c>
+      <c r="D6" t="n">
+        <v>39</v>
+      </c>
+      <c r="E6" t="n">
+        <v>29</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Best Coding Languages to Learn in 2019 - By Rafi Zikavashvili</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>https://hackernoon.com/best-coding-languages-to-learn-in-2019-b49b49250a25</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C7" t="n">
         <v>20</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D7" t="n">
         <v>2</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E7" t="n">
         <v>7</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t xml:space="preserve">support@hackernoon.com
 </t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>What Programming Language Should a Beginner Learn in 2019? | Codementor</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://www.codementor.io/codementorteam/beginner-programming-language-job-salary-community-7s26wmbm6</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>68</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" t="n">
-        <v>24</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Which Programming Language Should You Learn Next?</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://www.freecodecamp.org/news/which-programming-language-should-you-learn-next-487d077baa32/</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>12</v>
-      </c>
-      <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="n">
-        <v>9</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
-    </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
@@ -1273,29 +1304,24 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Google plus</t>
+          <t>Guide to Programming Languages | ComputerScience.org</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://raygun.com/blog/programming-languages/</t>
+          <t>https://www.computerscience.org/resources/computer-programming-languages/</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">example@xyz.com
-</t>
-        </is>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1327,44 +1353,44 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10 Best Programming Language to Learn in 2019</t>
+          <t>C Java Javascript C# Python C++ Ruby PHP Jobs, Employment | Indeed.com</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.guru99.com/best-programming-language.html</t>
+          <t>https://www.indeed.com/jobs?q=C+Java+Javascript+C%23+Python+C%2B%2B+Ruby+PHP</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8</v>
+        <v>1384</v>
       </c>
       <c r="D11" t="n">
         <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>C Java Javascript C# Python C++ Ruby PHP Jobs, Employment | Indeed.com</t>
+          <t>10 Best Programming Language to Learn in 2019</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/jobs?q=C+Java+Javascript+C%23+Python+C%2B%2B+Ruby+PHP</t>
+          <t>https://www.guru99.com/best-programming-language.html</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1396</v>
+        <v>8</v>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F12" t="inlineStr"/>
     </row>
@@ -1393,132 +1419,132 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Javascript C++ Jobs, Employment | Indeed.com</t>
+          <t>10 Best Programming Languages to Learn in 2019 (for Job &amp; Future)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/q-Javascript-C++-jobs.html</t>
+          <t>https://hackr.io/blog/best-programming-languages-to-learn-2019-jobs-future</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1581</v>
+        <v>63</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E14" t="n">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>An intro to 15 of the most important coding languages</t>
+          <t>The Best Programming Languages for each Situation</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://mashable.com/2015/12/05/learning-to-code/</t>
+          <t>https://tomassetti.me/best-programming-languages/</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D15" t="n">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="E15" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Warning: Your programming career - SoloLearn - Medium</t>
+          <t>Best Programming Languages to Learn: Choosing the Right One</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://medium.com/sololearn/warning-your-programming-career-b9579b3a878b</t>
+          <t>https://www.simplilearn.com/best-programming-languages-start-learning-today-article</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D16" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E16" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>The Best Programming Languages for each Situation</t>
+          <t>Programming Languages for Beginners: Understand All The Basics</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://tomassetti.me/best-programming-languages/</t>
+          <t>https://studywebdevelopment.com/programming-languages-for-beginners.html</t>
         </is>
       </c>
       <c r="C17" t="n">
         <v>8</v>
       </c>
       <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
         <v>4</v>
-      </c>
-      <c r="E17" t="n">
-        <v>34</v>
       </c>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>The 7 Most In-Demand Programming Languages of 2019 - Coding Dojo Blog</t>
+          <t>Top 10 Programming Languages for Engineers</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.codingdojo.com/blog/the-7-most-in-demand-programming-languages-of-2019</t>
+          <t>https://interestingengineering.com/top-10-programming-languages-for-engineers</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="D18" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E18" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>10 Best Programming Languages to Learn in 2019 (for Job &amp; Future)</t>
+          <t>twitter logo</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://hackr.io/blog/best-programming-languages-to-learn-2019-jobs-future</t>
+          <t>https://dev.to/javinpaul/why-java-is-the-best-programming-language-to-learn-coding-for-beginners-n89</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D19" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F19" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
started to add assertions and reformatted some items
</commit_message>
<xml_diff>
--- a/Excel_Data.xlsx
+++ b/Excel_Data.xlsx
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D6" t="n">
         <v>7</v>
@@ -677,45 +677,108 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Up For Grabs</t>
+          <t>10 Best Freelance Tcp Developers for Hire in Dec 2019 | Arc</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://up-for-grabs.net/</t>
+          <t>https://www.codementor.io/tcp-developers</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Making Sense of the Metadata: Clustering 4,000 Stack Overflow tags with BigQuery k-means - Stack Overflow Blog</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://stackoverflow.blog/2019/07/24/making-sense-of-the-metadata-clustering-4000-stack-overflow-tags-with-bigquery-k-means/</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>48</v>
+      </c>
+      <c r="D9" t="n">
+        <v>9</v>
+      </c>
+      <c r="E9" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>GitHub - quozd/awesome-dotnet: A collection of awesome .NET libraries, tools, frameworks and software</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://github.com/quozd/awesome-dotnet</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Access Denied</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/c-plus-plus-developer-jobs-in-kolkata</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>Remote C++ Jobs in December 2019</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>https://remoteok.io/remote-c-plus-plus-jobs</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C12" t="n">
         <v>11220</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D12" t="n">
         <v>79</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E12" t="n">
         <v>775</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t xml:space="preserve">hello@geektastic.com
 jobs@alienskin.com
@@ -725,48 +788,27 @@
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Making Sense of the Metadata: Clustering 4,000 Stack Overflow tags with BigQuery k-means - Stack Overflow Blog</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>https://stackoverflow.blog/2019/07/24/making-sense-of-the-metadata-clustering-4000-stack-overflow-tags-with-bigquery-k-means/</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>48</v>
-      </c>
-      <c r="D10" t="n">
-        <v>9</v>
-      </c>
-      <c r="E10" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="13">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Remote Software Developer Jobs in December 2019</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>https://remoteok.io/remote-dev-jobs</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C13" t="n">
         <v>11080</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D13" t="n">
         <v>90</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E13" t="n">
         <v>1617</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t xml:space="preserve">hello@geektastic.com
 talent@tuftandneedle.com
@@ -778,90 +820,94 @@
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Access Denied</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>https://www.naukri.com/c-plus-plus-developer-jobs-in-kolkata</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>GitHub - quozd/awesome-dotnet: A collection of awesome .NET libraries, tools, frameworks and software</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>https://github.com/quozd/awesome-dotnet</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>8</v>
-      </c>
-      <c r="D13" t="n">
-        <v>5</v>
-      </c>
-      <c r="E13" t="n">
-        <v>5</v>
-      </c>
-    </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>10 Best Freelance Tcp Developers for Hire in Dec 2019 | Arc</t>
+          <t xml:space="preserve">
+	Video Game, Animation, VFX and Software Jobs matching technical support in  - CreativeHeads.net
+</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.codementor.io/tcp-developers</t>
+          <t>https://www.creativeheads.net/job-search/technical-support/everywhere/3</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>104</v>
+        <v>1037</v>
       </c>
       <c r="D14" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t xml:space="preserve">
+	Video Game, Animation, VFX and Software Jobs matching cc++java in  - CreativeHeads.net
+</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://www.highendcareers.com/job-search/ccplusplusjava/everywhere/1</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1164</v>
+      </c>
+      <c r="D15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E15" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Should C# or C++ be chosen for learning Games Programming (consoles)? - Stack Overflow</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://stackoverflow.com/questions/2203093/should-c-sharp-or-c-be-chosen-for-learning-games-programming-consoles</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>64</v>
+      </c>
+      <c r="D16" t="n">
+        <v>7</v>
+      </c>
+      <c r="E16" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>Ask HN: Who wants to be hired? (April 2019) | Hacker News</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>https://news.ycombinator.com/item?id=19543938</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="C17" t="n">
         <v>50</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D17" t="n">
         <v>26</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E17" t="n">
         <v>323</v>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t xml:space="preserve">nathompson7@protonmail.com
 pcombs@gmail.com
@@ -996,71 +1042,25 @@
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Should C# or C++ be chosen for learning Games Programming (consoles)? - Stack Overflow</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>https://stackoverflow.com/questions/2203093/should-c-sharp-or-c-be-chosen-for-learning-games-programming-consoles</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>62</v>
-      </c>
-      <c r="D16" t="n">
-        <v>7</v>
-      </c>
-      <c r="E16" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-	Video Game, Animation, VFX and Software Jobs matching cc++java in  - CreativeHeads.net
-</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>https://www.highendcareers.com/job-search/ccplusplusjava/everywhere/1</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>1164</v>
-      </c>
-      <c r="D17" t="n">
-        <v>6</v>
-      </c>
-      <c r="E17" t="n">
-        <v>80</v>
-      </c>
-    </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-	Video Game, Animation, VFX and Software Jobs matching technical support in  - CreativeHeads.net
-</t>
+          <t>Tech recruiters’ search tool for exploring IT terms</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.creativeheads.net/job-search/technical-support/everywhere/3</t>
+          <t>https://glossarytech.com/search/results?phrase=.NET%20Core.html</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1036</v>
+        <v>26</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="E18" t="n">
-        <v>95</v>
+        <v>284</v>
       </c>
     </row>
     <row r="19">
@@ -1167,117 +1167,117 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Warning: Your programming career - SoloLearn - Medium</t>
+          <t>What Programming Language Should a Beginner Learn in 2019? | Codementor</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://medium.com/sololearn/warning-your-programming-career-b9579b3a878b</t>
+          <t>https://www.codementor.io/codementorteam/beginner-programming-language-job-salary-community-7s26wmbm6</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>What Programming Language Should a Beginner Learn in 2019? | Codementor</t>
+          <t>Top 10 Programming Languages of the World – 2019 to begin with… - GeeksforGeeks</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.codementor.io/codementorteam/beginner-programming-language-job-salary-community-7s26wmbm6</t>
+          <t>https://www.geeksforgeeks.org/top-10-programming-languages-of-the-world-2019-to-begin-with/</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="E4" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>The 7 Most In-Demand Programming Languages of 2019 - Coding Dojo Blog</t>
+          <t>Warning: Your programming career - SoloLearn - Medium</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.codingdojo.com/blog/the-7-most-in-demand-programming-languages-of-2019</t>
+          <t>https://medium.com/sololearn/warning-your-programming-career-b9579b3a878b</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E5" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Top 10 Programming Languages of the World – 2019 to begin with… - GeeksforGeeks</t>
+          <t>Best Coding Languages to Learn in 2019 - By Rafi Zikavashvili</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.geeksforgeeks.org/top-10-programming-languages-of-the-world-2019-to-begin-with/</t>
+          <t>https://hackernoon.com/best-coding-languages-to-learn-in-2019-b49b49250a25</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D6" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>29</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">support@hackernoon.com
+</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Best Coding Languages to Learn in 2019 - By Rafi Zikavashvili</t>
+          <t>The 7 Most In-Demand Programming Languages of 2019 - Coding Dojo Blog</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://hackernoon.com/best-coding-languages-to-learn-in-2019-b49b49250a25</t>
+          <t>https://www.codingdojo.com/blog/the-7-most-in-demand-programming-languages-of-2019</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">support@hackernoon.com
-</t>
-        </is>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1304,93 +1304,93 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Guide to Programming Languages | ComputerScience.org</t>
+          <t>The 9 Best Programming Languages to Learn in 2019 | Fullstack Academy</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.computerscience.org/resources/computer-programming-languages/</t>
+          <t>https://www.fullstackacademy.com/blog/nine-best-programming-languages-to-learn-2018</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D9" t="n">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="E9" t="n">
-        <v>29</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
+        <v>13</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@fullstackacademy.com
+</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>The 9 Best Programming Languages to Learn in 2019 | Fullstack Academy</t>
+          <t>Guide to Programming Languages | ComputerScience.org</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.fullstackacademy.com/blog/nine-best-programming-languages-to-learn-2018</t>
+          <t>https://www.computerscience.org/resources/computer-programming-languages/</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D10" t="n">
-        <v>6</v>
+        <v>122</v>
       </c>
       <c r="E10" t="n">
-        <v>13</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">hello@fullstackacademy.com
-</t>
-        </is>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>C Java Javascript C# Python C++ Ruby PHP Jobs, Employment | Indeed.com</t>
+          <t>10 Best Programming Languages to Learn in 2019 (for Job &amp; Future)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/jobs?q=C+Java+Javascript+C%23+Python+C%2B%2B+Ruby+PHP</t>
+          <t>https://hackr.io/blog/best-programming-languages-to-learn-2019-jobs-future</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1384</v>
+        <v>63</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E11" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>10 Best Programming Language to Learn in 2019</t>
+          <t>C Java Javascript C# Python C++ Ruby PHP Jobs, Employment | Indeed.com</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.guru99.com/best-programming-language.html</t>
+          <t>https://www.indeed.com/jobs?q=C+Java+Javascript+C%23+Python+C%2B%2B+Ruby+PHP</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8</v>
+        <v>1344</v>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F12" t="inlineStr"/>
     </row>
@@ -1419,66 +1419,66 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>10 Best Programming Languages to Learn in 2019 (for Job &amp; Future)</t>
+          <t>10 Best Programming Language to Learn in 2019</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://hackr.io/blog/best-programming-languages-to-learn-2019-jobs-future</t>
+          <t>https://www.guru99.com/best-programming-language.html</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="D14" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>The Best Programming Languages for each Situation</t>
+          <t>Best Programming Languages to Learn: Choosing the Right One</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://tomassetti.me/best-programming-languages/</t>
+          <t>https://www.simplilearn.com/best-programming-languages-start-learning-today-article</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E15" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Best Programming Languages to Learn: Choosing the Right One</t>
+          <t>The Best Programming Languages for each Situation</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.simplilearn.com/best-programming-languages-start-learning-today-article</t>
+          <t>https://tomassetti.me/best-programming-languages/</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D16" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="F16" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Polished up the code and added comments
</commit_message>
<xml_diff>
--- a/Excel_Data.xlsx
+++ b/Excel_Data.xlsx
@@ -1002,75 +1002,75 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Access to this page has been denied.</t>
+          <t>netguru_logo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.upwork.com/l/cn/python-developers/</t>
+          <t>https://www.netguru.com/blog/python-vs-c-comparison-of-the-programming-language</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@netguru.com
+hello@netguru.com
+</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>14 Programming Languages for Mobile App Development - BuildFire</t>
+          <t>Access to this page has been denied.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://buildfire.com/programming-languages-for-mobile-app-development/</t>
+          <t>https://www.upwork.com/l/cn/python-developers/</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>17</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">johndoe@example.com
-</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>netguru_logo</t>
+          <t>Google plus</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.netguru.com/blog/python-vs-c-comparison-of-the-programming-language</t>
+          <t>https://raygun.com/blog/programming-languages/</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello@netguru.com
-hello@netguru.com
+          <t xml:space="preserve">example@xyz.com
 </t>
         </is>
       </c>
@@ -1078,156 +1078,295 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Google plus</t>
+          <t>C++ Vs. C# - What’s the Difference?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://raygun.com/blog/programming-languages/</t>
+          <t>https://www.guru99.com/cpp-vs-c-sharp.html</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">example@xyz.com
-</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>C++ Vs. C# - What’s the Difference?</t>
+          <t>14 Programming Languages for Mobile App Development - BuildFire</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.guru99.com/cpp-vs-c-sharp.html</t>
+          <t>https://buildfire.com/programming-languages-for-mobile-app-development/</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">johndoe@example.com
+</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Up For Grabs</t>
+          <t>Visual Studio for Linux - Developer Community</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://up-for-grabs.net/</t>
+          <t>https://developercommunity.visualstudio.com/idea/360479/visual-studio-for-linux.html</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">shunjid.se@outlook.com
+shunjid.se@outlook.com
+</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>403 Forbidden</t>
+          <t>Up For Grabs</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.beseen.com/tech-jobs/roles/software-developer.html</t>
+          <t>https://up-for-grabs.net/</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Should C# or C++ be chosen for learning Games Programming (consoles)? - Stack Overflow</t>
+          <t>Making Sense of the Metadata: Clustering 4,000 Stack Overflow tags with BigQuery k-means - Stack Overflow Blog</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/questions/2203093/should-c-sharp-or-c-be-chosen-for-learning-games-programming-consoles</t>
+          <t>https://stackoverflow.blog/2019/07/24/making-sense-of-the-metadata-clustering-4000-stack-overflow-tags-with-bigquery-k-means/</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D9" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E9" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Making Sense of the Metadata: Clustering 4,000 Stack Overflow tags with BigQuery k-means - Stack Overflow Blog</t>
+          <t>Remote Software Developer Jobs in December 2019</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://stackoverflow.blog/2019/07/24/making-sense-of-the-metadata-clustering-4000-stack-overflow-tags-with-bigquery-k-means/</t>
+          <t>https://remoteok.io/remote-dev-jobs</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>48</v>
+        <v>10880</v>
       </c>
       <c r="D10" t="n">
-        <v>9</v>
+        <v>94</v>
       </c>
       <c r="E10" t="n">
-        <v>12</v>
+        <v>1534</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@geektastic.com
+talent@tuftandneedle.com
+sentinelhr@sentinel.com
+jobs@wpwhitesecurity.com
+alise.moncure@integratedrental.com
+alise.moncure@integratedrental.com
+</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Remote C++ Jobs in December 2019</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://remoteok.io/remote-c-plus-plus-jobs</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>11167</v>
+      </c>
+      <c r="D11" t="n">
+        <v>79</v>
+      </c>
+      <c r="E11" t="n">
+        <v>767</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@geektastic.com
+jobs@alienskin.com
+schuss@madeinoffice.com
+jobs@komodoplatform.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Which is better for programming, a Mac or Windows laptop? - Quora</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://www.quora.com/Which-is-better-for-programming-a-Mac-or-Windows-laptop</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>15</v>
+      </c>
+      <c r="D12" t="n">
+        <v>14</v>
+      </c>
+      <c r="E12" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>GitHub - uhub/awesome-cpp: A curated list of awesome C++ frameworks, libraries and software.</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://github.com/uhub/awesome-cpp</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" t="n">
+        <v>19</v>
+      </c>
+      <c r="E13" t="n">
+        <v>49</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sean@seanstarkey.com
+sean@seanstarkey.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>What is the difference between C, C++ and C#? - Quora</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://www.quora.com/What-is-the-difference-between-C-C++-and-C</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>9</v>
+      </c>
+      <c r="D14" t="n">
+        <v>9</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Should C# or C++ be chosen for learning Games Programming (consoles)? - Stack Overflow</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://stackoverflow.com/questions/2203093/should-c-sharp-or-c-be-chosen-for-learning-games-programming-consoles</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>62</v>
+      </c>
+      <c r="D15" t="n">
+        <v>8</v>
+      </c>
+      <c r="E15" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>Ask HN: Who wants to be hired? (April 2019) | Hacker News</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>https://news.ycombinator.com/item?id=19543938</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C16" t="n">
         <v>50</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D16" t="n">
         <v>26</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E16" t="n">
         <v>323</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t xml:space="preserve">nathompson7@protonmail.com
 pcombs@gmail.com
@@ -1362,164 +1501,25 @@
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>What is the difference between C, C++ and C#? - Quora</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>https://www.quora.com/What-is-the-difference-between-C-C++-and-C</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>9</v>
-      </c>
-      <c r="D12" t="n">
-        <v>9</v>
-      </c>
-      <c r="E12" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>GitHub - uhub/awesome-cpp: A curated list of awesome C++ frameworks, libraries and software.</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>https://github.com/uhub/awesome-cpp</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>12</v>
-      </c>
-      <c r="D13" t="n">
-        <v>19</v>
-      </c>
-      <c r="E13" t="n">
-        <v>49</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sean@seanstarkey.com
-sean@seanstarkey.com
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Visual Studio for Linux - Developer Community</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>https://developercommunity.visualstudio.com/idea/360479/visual-studio-for-linux.html</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>12</v>
-      </c>
-      <c r="D14" t="n">
-        <v>4</v>
-      </c>
-      <c r="E14" t="n">
-        <v>29</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">shunjid.se@outlook.com
-shunjid.se@outlook.com
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Which is better for programming, a Mac or Windows laptop? - Quora</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>https://www.quora.com/Which-is-better-for-programming-a-Mac-or-Windows-laptop</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>15</v>
-      </c>
-      <c r="D15" t="n">
-        <v>16</v>
-      </c>
-      <c r="E15" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Remote Software Developer Jobs in December 2019</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>https://remoteok.io/remote-dev-jobs</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>10809</v>
-      </c>
-      <c r="D16" t="n">
-        <v>90</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1536</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">hello@geektastic.com
-talent@tuftandneedle.com
-sentinelhr@sentinel.com
-jobs@wpwhitesecurity.com
-alise.moncure@integratedrental.com
-alise.moncure@integratedrental.com
-</t>
-        </is>
-      </c>
-    </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Remote C++ Jobs in December 2019</t>
+          <t>403 Forbidden</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://remoteok.io/remote-c-plus-plus-jobs</t>
+          <t>https://www.beseen.com/tech-jobs/roles/software-developer.html</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>11167</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>767</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">hello@geektastic.com
-jobs@alienskin.com
-schuss@madeinoffice.com
-jobs@komodoplatform.com
-</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1626,24 +1626,90 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>The 7 Most In-Demand Programming Languages of 2019 - Coding Dojo Blog</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://www.codingdojo.com/blog/the-7-most-in-demand-programming-languages-of-2019</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>59</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>11</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>What Programming Language Should a Beginner Learn in 2019? | Codementor</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://www.codementor.io/codementorteam/beginner-programming-language-job-salary-community-7s26wmbm6</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>68</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Warning: Your programming career - SoloLearn - Medium</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://medium.com/sololearn/warning-your-programming-career-b9579b3a878b</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>54</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" t="n">
+        <v>20</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>Thinkful Logo Black@2x</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>https://www.thinkful.com/blog/what-programming-language-should-you-learn-according-to-your-state/</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C6" t="n">
         <v>11</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D6" t="n">
         <v>0</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E6" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t xml:space="preserve">tatiana@thinkful.com
 tatiana@thinkful.com
@@ -1655,144 +1721,73 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Warning: Your programming career - SoloLearn - Medium</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://medium.com/sololearn/warning-your-programming-career-b9579b3a878b</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>54</v>
-      </c>
-      <c r="D4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" t="n">
-        <v>20</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Top 10 Programming Languages of the World – 2019 to begin with… - GeeksforGeeks</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>https://www.geeksforgeeks.org/top-10-programming-languages-of-the-world-2019-to-begin-with/</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>28</v>
-      </c>
-      <c r="D5" t="n">
-        <v>41</v>
-      </c>
-      <c r="E5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>hello</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://dev.to/javinpaul/top-5-programming-languages-every-software-developer-should-learn-3o3o</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>14</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
-    </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Best Coding Languages to Learn in 2019 - By Rafi Zikavashvili</t>
+          <t>Top 10 Programming Languages of the World – 2019 to begin with… - GeeksforGeeks</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://hackernoon.com/best-coding-languages-to-learn-in-2019-b49b49250a25</t>
+          <t>https://www.geeksforgeeks.org/top-10-programming-languages-of-the-world-2019-to-begin-with/</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">support@hackernoon.com
-</t>
-        </is>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>The 5 Most Popular Programming Languages of 2019</t>
+          <t>Which Programming Language Should You Learn Next?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://stackify.com/popular-programming-languages-2018/</t>
+          <t>https://www.freecodecamp.org/news/which-programming-language-should-you-learn-next-487d077baa32/</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Google plus</t>
+          <t>Best Coding Languages to Learn in 2019 - By Rafi Zikavashvili</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://raygun.com/blog/programming-languages/</t>
+          <t>https://hackernoon.com/best-coding-languages-to-learn-in-2019-b49b49250a25</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve">example@xyz.com
+          <t xml:space="preserve">support@hackernoon.com
 </t>
         </is>
       </c>
@@ -1800,137 +1795,137 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>The 9 Best Programming Languages to Learn in 2019 | Fullstack Academy</t>
+          <t>The 5 Most Popular Programming Languages of 2019</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.fullstackacademy.com/blog/nine-best-programming-languages-to-learn-2018</t>
+          <t>https://stackify.com/popular-programming-languages-2018/</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D10" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>15</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">hello@fullstackacademy.com
-</t>
-        </is>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>C Java Javascript C# Python C++ Ruby PHP Jobs, Employment | Indeed.com</t>
+          <t>hello</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/jobs?q=C+Java+Javascript+C%23+Python+C%2B%2B+Ruby+PHP</t>
+          <t>https://dev.to/javinpaul/top-5-programming-languages-every-software-developer-should-learn-3o3o</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1387</v>
+        <v>14</v>
       </c>
       <c r="D11" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Javascript C++ Jobs, Employment | Indeed.com</t>
+          <t>10 Best Programming Languages to Learn in 2019 (for Job &amp; Future)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/q-Javascript-C++-jobs.html</t>
+          <t>https://hackr.io/blog/best-programming-languages-to-learn-2019-jobs-future</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1792</v>
+        <v>59</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E12" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>What Programming Language Should a Beginner Learn in 2019? | Codementor</t>
+          <t>Javascript C++ Jobs, Employment | Indeed.com</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.codementor.io/codementorteam/beginner-programming-language-job-salary-community-7s26wmbm6</t>
+          <t>https://www.indeed.com/q-Javascript-C++-jobs.html</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>68</v>
+        <v>1582</v>
       </c>
       <c r="D13" t="n">
         <v>2</v>
       </c>
       <c r="E13" t="n">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>An intro to 15 of the most important coding languages</t>
+          <t>Google plus</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://mashable.com/2015/12/05/learning-to-code/</t>
+          <t>https://raygun.com/blog/programming-languages/</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>25</v>
+        <v>127</v>
       </c>
       <c r="D14" t="n">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>32</v>
-      </c>
-      <c r="F14" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">example@xyz.com
+</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>10 Best Programming Language to Learn in 2020</t>
+          <t>C Java Javascript C# Python C++ Ruby PHP Jobs, Employment | Indeed.com</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.guru99.com/best-programming-language.html</t>
+          <t>https://www.indeed.com/jobs?q=C+Java+Javascript+C%23+Python+C%2B%2B+Ruby+PHP</t>
         </is>
       </c>
       <c r="C15" t="n">
+        <v>1534</v>
+      </c>
+      <c r="D15" t="n">
         <v>8</v>
       </c>
-      <c r="D15" t="n">
-        <v>3</v>
-      </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F15" t="inlineStr"/>
     </row>
@@ -1959,66 +1954,71 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>The 7 Most In-Demand Programming Languages of 2019 - Coding Dojo Blog</t>
+          <t>The 9 Best Programming Languages to Learn in 2019 | Fullstack Academy</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.codingdojo.com/blog/the-7-most-in-demand-programming-languages-of-2019</t>
+          <t>https://www.fullstackacademy.com/blog/nine-best-programming-languages-to-learn-2018</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E17" t="n">
-        <v>11</v>
-      </c>
-      <c r="F17" t="inlineStr"/>
+        <v>15</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@fullstackacademy.com
+</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>10 Best Programming Languages to Learn in 2019 (for Job &amp; Future)</t>
+          <t>10 Best Programming Language to Learn in 2020</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://hackr.io/blog/best-programming-languages-to-learn-2019-jobs-future</t>
+          <t>https://www.guru99.com/best-programming-language.html</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="D18" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Which Programming Language Should You Learn Next?</t>
+          <t>An intro to 15 of the most important coding languages</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.freecodecamp.org/news/which-programming-language-should-you-learn-next-487d077baa32/</t>
+          <t>https://mashable.com/2015/12/05/learning-to-code/</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F19" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Polished up code more
</commit_message>
<xml_diff>
--- a/Excel_Data.xlsx
+++ b/Excel_Data.xlsx
@@ -1030,49 +1030,49 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Access to this page has been denied.</t>
+          <t>Google plus</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.upwork.com/l/cn/python-developers/</t>
+          <t>https://raygun.com/blog/programming-languages/</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">example@xyz.com
+</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Google plus</t>
+          <t>Access to this page has been denied.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://raygun.com/blog/programming-languages/</t>
+          <t>https://www.upwork.com/l/cn/python-developers/</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">example@xyz.com
-</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1196,24 +1196,54 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Remote C++ Jobs in December 2019</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://remoteok.io/remote-c-plus-plus-jobs</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>11167</v>
+      </c>
+      <c r="D10" t="n">
+        <v>79</v>
+      </c>
+      <c r="E10" t="n">
+        <v>767</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@geektastic.com
+jobs@alienskin.com
+schuss@madeinoffice.com
+jobs@komodoplatform.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>Remote Software Developer Jobs in December 2019</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>https://remoteok.io/remote-dev-jobs</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C11" t="n">
         <v>10880</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>94</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E11" t="n">
         <v>1534</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t xml:space="preserve">hello@geektastic.com
 talent@tuftandneedle.com
@@ -1225,148 +1255,55 @@
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Remote C++ Jobs in December 2019</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>https://remoteok.io/remote-c-plus-plus-jobs</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>11167</v>
-      </c>
-      <c r="D11" t="n">
-        <v>79</v>
-      </c>
-      <c r="E11" t="n">
-        <v>767</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">hello@geektastic.com
-jobs@alienskin.com
-schuss@madeinoffice.com
-jobs@komodoplatform.com
-</t>
-        </is>
-      </c>
-    </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Which is better for programming, a Mac or Windows laptop? - Quora</t>
+          <t>GitHub - uhub/awesome-cpp: A curated list of awesome C++ frameworks, libraries and software.</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.quora.com/Which-is-better-for-programming-a-Mac-or-Windows-laptop</t>
+          <t>https://github.com/uhub/awesome-cpp</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D12" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E12" t="n">
-        <v>16</v>
+        <v>49</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sean@seanstarkey.com
+sean@seanstarkey.com
+</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GitHub - uhub/awesome-cpp: A curated list of awesome C++ frameworks, libraries and software.</t>
+          <t>Ask HN: Who wants to be hired? (April 2019) | Hacker News</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://github.com/uhub/awesome-cpp</t>
+          <t>https://news.ycombinator.com/item?id=19543938</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D13" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E13" t="n">
-        <v>49</v>
+        <v>323</v>
       </c>
       <c r="F13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sean@seanstarkey.com
-sean@seanstarkey.com
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>What is the difference between C, C++ and C#? - Quora</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>https://www.quora.com/What-is-the-difference-between-C-C++-and-C</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>9</v>
-      </c>
-      <c r="D14" t="n">
-        <v>9</v>
-      </c>
-      <c r="E14" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Should C# or C++ be chosen for learning Games Programming (consoles)? - Stack Overflow</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>https://stackoverflow.com/questions/2203093/should-c-sharp-or-c-be-chosen-for-learning-games-programming-consoles</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>62</v>
-      </c>
-      <c r="D15" t="n">
-        <v>8</v>
-      </c>
-      <c r="E15" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Ask HN: Who wants to be hired? (April 2019) | Hacker News</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>https://news.ycombinator.com/item?id=19543938</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>50</v>
-      </c>
-      <c r="D16" t="n">
-        <v>26</v>
-      </c>
-      <c r="E16" t="n">
-        <v>323</v>
-      </c>
-      <c r="F16" t="inlineStr">
         <is>
           <t xml:space="preserve">nathompson7@protonmail.com
 pcombs@gmail.com
@@ -1501,25 +1438,88 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Should C# or C++ be chosen for learning Games Programming (consoles)? - Stack Overflow</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://stackoverflow.com/questions/2203093/should-c-sharp-or-c-be-chosen-for-learning-games-programming-consoles</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>62</v>
+      </c>
+      <c r="D14" t="n">
+        <v>7</v>
+      </c>
+      <c r="E14" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>What is the difference between C, C++ and C#? - Quora</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://www.quora.com/What-is-the-difference-between-C-C++-and-C</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>9</v>
+      </c>
+      <c r="D15" t="n">
+        <v>9</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>C++ Rest Sdk Linux</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://rtmm.ts-fliesenservice.de/c++-rest-sdk-linux.html</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8</v>
+      </c>
+    </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>403 Forbidden</t>
+          <t>Which is better for programming, a Mac or Windows laptop? - Quora</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.beseen.com/tech-jobs/roles/software-developer.html</t>
+          <t>https://www.quora.com/Which-is-better-for-programming-a-Mac-or-Windows-laptop</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18">
@@ -1626,90 +1626,112 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>The 7 Most In-Demand Programming Languages of 2019 - Coding Dojo Blog</t>
+          <t>Warning: Your programming career - SoloLearn - Medium</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.codingdojo.com/blog/the-7-most-in-demand-programming-languages-of-2019</t>
+          <t>https://medium.com/sololearn/warning-your-programming-career-b9579b3a878b</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>What Programming Language Should a Beginner Learn in 2019? | Codementor</t>
+          <t>The 7 Most In-Demand Programming Languages of 2019 - Coding Dojo Blog</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.codementor.io/codementorteam/beginner-programming-language-job-salary-community-7s26wmbm6</t>
+          <t>https://www.codingdojo.com/blog/the-7-most-in-demand-programming-languages-of-2019</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Warning: Your programming career - SoloLearn - Medium</t>
+          <t>Which Programming Language Should You Learn Next?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://medium.com/sololearn/warning-your-programming-career-b9579b3a878b</t>
+          <t>https://www.freecodecamp.org/news/which-programming-language-should-you-learn-next-487d077baa32/</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Top 10 Programming Languages of the World – 2019 to begin with… - GeeksforGeeks</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.geeksforgeeks.org/top-10-programming-languages-of-the-world-2019-to-begin-with/</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>28</v>
+      </c>
+      <c r="D6" t="n">
+        <v>41</v>
+      </c>
+      <c r="E6" t="n">
+        <v>29</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Thinkful Logo Black@2x</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>https://www.thinkful.com/blog/what-programming-language-should-you-learn-according-to-your-state/</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C7" t="n">
         <v>11</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D7" t="n">
         <v>0</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t xml:space="preserve">tatiana@thinkful.com
 tatiana@thinkful.com
@@ -1721,47 +1743,25 @@
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Top 10 Programming Languages of the World – 2019 to begin with… - GeeksforGeeks</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://www.geeksforgeeks.org/top-10-programming-languages-of-the-world-2019-to-begin-with/</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>28</v>
-      </c>
-      <c r="D7" t="n">
-        <v>41</v>
-      </c>
-      <c r="E7" t="n">
-        <v>29</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
-    </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Which Programming Language Should You Learn Next?</t>
+          <t>What Programming Language Should a Beginner Learn in 2019? | Codementor</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.freecodecamp.org/news/which-programming-language-should-you-learn-next-487d077baa32/</t>
+          <t>https://www.codementor.io/codementorteam/beginner-programming-language-job-salary-community-7s26wmbm6</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F8" t="inlineStr"/>
     </row>
@@ -1861,51 +1861,51 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Javascript C++ Jobs, Employment | Indeed.com</t>
+          <t>Google plus</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/q-Javascript-C++-jobs.html</t>
+          <t>https://raygun.com/blog/programming-languages/</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1582</v>
+        <v>127</v>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>37</v>
-      </c>
-      <c r="F13" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">example@xyz.com
+</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Google plus</t>
+          <t>Javascript C++ Jobs, Employment | Indeed.com</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://raygun.com/blog/programming-languages/</t>
+          <t>https://www.indeed.com/q-Javascript-C++-jobs.html</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>127</v>
+        <v>1595</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">example@xyz.com
-</t>
-        </is>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1919,64 +1919,64 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1534</v>
+        <v>1537</v>
       </c>
       <c r="D15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>The Best Programming Languages for each Situation</t>
+          <t>The 9 Best Programming Languages to Learn in 2019 | Fullstack Academy</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://tomassetti.me/best-programming-languages/</t>
+          <t>https://www.fullstackacademy.com/blog/nine-best-programming-languages-to-learn-2018</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D16" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E16" t="n">
-        <v>34</v>
-      </c>
-      <c r="F16" t="inlineStr"/>
+        <v>15</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@fullstackacademy.com
+</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>The 9 Best Programming Languages to Learn in 2019 | Fullstack Academy</t>
+          <t>The Best Programming Languages for each Situation</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.fullstackacademy.com/blog/nine-best-programming-languages-to-learn-2018</t>
+          <t>https://tomassetti.me/best-programming-languages/</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D17" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E17" t="n">
-        <v>15</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">hello@fullstackacademy.com
-</t>
-        </is>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">

</xml_diff>